<commit_message>
work on localconf mechanism
</commit_message>
<xml_diff>
--- a/notes/local settings database structure.xlsx
+++ b/notes/local settings database structure.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBF8369-85F3-4CAE-8C89-CB8215519141}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A482F1EB-06EB-4069-B5C4-B1538E9F7775}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="local settings" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>table</t>
   </si>
@@ -37,9 +37,6 @@
     <t>values</t>
   </si>
   <si>
-    <t>passwords</t>
-  </si>
-  <si>
     <t>pool</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>NULL if password applies to VFS itself</t>
   </si>
   <si>
-    <t>local</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
@@ -79,7 +73,22 @@
     <t>value4</t>
   </si>
   <si>
-    <t>value5</t>
+    <t>storagepass</t>
+  </si>
+  <si>
+    <t>localconf</t>
+  </si>
+  <si>
+    <t>value0</t>
+  </si>
+  <si>
+    <t>base64-encoded</t>
+  </si>
+  <si>
+    <t>ALTER TABLE storagepass ADD CONSTRAINT onePasswordPerPool UNIQUE (vfs , pool)</t>
+  </si>
+  <si>
+    <t>ALTER TABLE localconf ADD CONSTRAINT oneValuesetPerKey UNIQUE (service , section , key)</t>
   </si>
 </sst>
 </file>
@@ -104,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +123,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -145,9 +160,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,21 +444,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="74.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="74.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,101 +475,114 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on localconf passwords
</commit_message>
<xml_diff>
--- a/notes/local settings database structure.xlsx
+++ b/notes/local settings database structure.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A482F1EB-06EB-4069-B5C4-B1538E9F7775}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7702BE99-D426-4540-8305-599A8549D8BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="local settings" sheetId="1" r:id="rId1"/>
@@ -85,10 +85,10 @@
     <t>base64-encoded</t>
   </si>
   <si>
-    <t>ALTER TABLE storagepass ADD CONSTRAINT onePasswordPerPool UNIQUE (vfs , pool)</t>
-  </si>
-  <si>
-    <t>ALTER TABLE localconf ADD CONSTRAINT oneValuesetPerKey UNIQUE (service , section , key)</t>
+    <t>UNIQUE (vfs , pool)</t>
+  </si>
+  <si>
+    <t>UNIQUE (service , section , key)</t>
   </si>
 </sst>
 </file>
@@ -113,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,12 +123,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,10 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,13 +440,13 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" customWidth="1"/>
     <col min="4" max="4" width="74.7109375" customWidth="1"/>
   </cols>
@@ -508,8 +501,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -580,8 +573,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>